<commit_message>
Viz Ready (except waffle, sankey, and regs)
</commit_message>
<xml_diff>
--- a/report_outline_v0.xlsx
+++ b/report_outline_v0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/Data Analytics/6. Country Reports/Qatar-Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4156" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D35887AB-6973-E14E-ACAC-A8B70E9C0DB4}"/>
+  <xr:revisionPtr revIDLastSave="4232" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCE177F2-C896-3F48-BF73-E3CB2F32FC8E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
   </bookViews>
   <sheets>
     <sheet name="general_info" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="292">
   <si>
     <t>Cover</t>
   </si>
@@ -480,12 +480,6 @@
     <t>Percentage of respondents who have a lot, some, little, or no trust in…</t>
   </si>
   <si>
-    <t>A lot, Some, DKNA, Little, No trust</t>
-  </si>
-  <si>
-    <t>#18538E, #46B5FF, #d8d8d8, #FFC818, #FF7900</t>
-  </si>
-  <si>
     <t>q1a</t>
   </si>
   <si>
@@ -528,12 +522,6 @@
     <t>Source: WJP General Population Poll 2026</t>
   </si>
   <si>
-    <t>#FF7900, #FFC818, #d8d8d8, #46B5FF, #18538E</t>
-  </si>
-  <si>
-    <t>All of them, Most of them, DKNA, Some of them, None</t>
-  </si>
-  <si>
     <t>Figure_3</t>
   </si>
   <si>
@@ -552,9 +540,6 @@
     <t>Diverging bars</t>
   </si>
   <si>
-    <t>#003b8a, #fa4d57</t>
-  </si>
-  <si>
     <t>Figure_4</t>
   </si>
   <si>
@@ -573,9 +558,6 @@
     <t>Qatari, Foreigner</t>
   </si>
   <si>
-    <t xml:space="preserve">#49178e, #dd58b1 </t>
-  </si>
-  <si>
     <t>Source: WJP General Population Poll 2027</t>
   </si>
   <si>
@@ -693,12 +675,6 @@
     <t>q48c_G2, EXP_q22i_G2, EXP_q22h_G2, q48a_G2, q48b_G2</t>
   </si>
   <si>
-    <t>q48a_G1, q48b_G1, EXP_q22e_G1, q48c_G1, q48d_G2</t>
-  </si>
-  <si>
-    <t>q48d_G1, EXP_q22f_G1, EXP_q22h_G1, EXP_q22k_G2, EXP_q22j_G2</t>
-  </si>
-  <si>
     <t>Percentage of people who agree or strongly agree that the police…</t>
   </si>
   <si>
@@ -832,6 +808,114 @@
   </si>
   <si>
     <t>q4a, q4b, q4c, q4d, q4e</t>
+  </si>
+  <si>
+    <t>1, 0</t>
+  </si>
+  <si>
+    <t>q48a_G1, q48b_G1, EXP_q22e_G1_inv, q48c_G1, q48d_G2</t>
+  </si>
+  <si>
+    <t>q48d_G1, EXP_q22f_G1, EXP_q22h_G1, EXP_q22k_G2_inv, EXP_q22j_G2_inv</t>
+  </si>
+  <si>
+    <t>trt1</t>
+  </si>
+  <si>
+    <t>trt2</t>
+  </si>
+  <si>
+    <t>trt3</t>
+  </si>
+  <si>
+    <t>cor1</t>
+  </si>
+  <si>
+    <t>cor2</t>
+  </si>
+  <si>
+    <t>cor3</t>
+  </si>
+  <si>
+    <t>acc1</t>
+  </si>
+  <si>
+    <t>cjs1</t>
+  </si>
+  <si>
+    <t>cja1</t>
+  </si>
+  <si>
+    <t>cja2</t>
+  </si>
+  <si>
+    <t>cja3</t>
+  </si>
+  <si>
+    <t>pol1</t>
+  </si>
+  <si>
+    <t>pol2</t>
+  </si>
+  <si>
+    <t>pol3</t>
+  </si>
+  <si>
+    <t>pol4</t>
+  </si>
+  <si>
+    <t>tcv1</t>
+  </si>
+  <si>
+    <t>pff1</t>
+  </si>
+  <si>
+    <t>cri1</t>
+  </si>
+  <si>
+    <t>cvr1</t>
+  </si>
+  <si>
+    <t>pos1</t>
+  </si>
+  <si>
+    <t>pos2</t>
+  </si>
+  <si>
+    <t>dis1</t>
+  </si>
+  <si>
+    <t>dis2</t>
+  </si>
+  <si>
+    <t>dis3</t>
+  </si>
+  <si>
+    <t>unique_id</t>
+  </si>
+  <si>
+    <t>#fa4d57, #003b8a</t>
+  </si>
+  <si>
+    <t>#49178e, #dd58b1</t>
+  </si>
+  <si>
+    <t>#2a2a94, #a90099, #3273ff</t>
+  </si>
+  <si>
+    <t>Prosecutors, Judges and magistrates, Public defense attorneys</t>
+  </si>
+  <si>
+    <t>#18538E, #46B5FF, #FFC818, #FF7900</t>
+  </si>
+  <si>
+    <t>A lot, Some, Little, No trust</t>
+  </si>
+  <si>
+    <t>All of them, Most of them, Some of them, None</t>
+  </si>
+  <si>
+    <t>#FF7900, #FFC818, #46B5FF, #18538E</t>
   </si>
 </sst>
 </file>
@@ -1362,10 +1446,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}" name="Table53" displayName="Table53" ref="A1:Q25" totalsRowShown="0" dataDxfId="29">
-  <autoFilter ref="A1:Q25" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}" name="Table53" displayName="Table53" ref="A1:R25" totalsRowShown="0" dataDxfId="29">
+  <autoFilter ref="A1:R25" xr:uid="{F4E522B1-3123-499E-83E5-BBB41A9C0B72}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{D92A50FF-F655-438A-821F-D4E0A6773705}" name="id" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{83BE05A7-E625-7D4B-B471-5B9EF89254A6}" name="unique_id"/>
     <tableColumn id="2" xr3:uid="{4F1F3430-F8D1-427E-BB79-2C98EFBD6FEE}" name="panel" dataDxfId="27"/>
     <tableColumn id="19" xr3:uid="{1520B749-B840-4CF5-8EF6-A17C6F7666CB}" name="chart_title" dataDxfId="26"/>
     <tableColumn id="20" xr3:uid="{1D6414BC-35AE-48B3-8DCF-B552D8374772}" name="chart_subtitle" dataDxfId="25"/>
@@ -1802,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B32341-F9AC-424D-8D69-9ABCF2FF7D4F}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2946,1347 +3031,1422 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942074E-1171-4680-A697-1A8E37014FFA}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="16" max="16" width="10.5" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="10.5" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
       <c r="B2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>145</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>143</v>
       </c>
-      <c r="F2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
-        <v>149</v>
-      </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
         <v>82</v>
       </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
       <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
         <v>144</v>
       </c>
-      <c r="M2" t="s">
-        <v>198</v>
-      </c>
       <c r="N2" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="O2" t="s">
-        <v>147</v>
+        <v>289</v>
       </c>
       <c r="P2" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
       <c r="C3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
         <v>142</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>145</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>143</v>
       </c>
-      <c r="F3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H3" t="s">
-        <v>156</v>
-      </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
         <v>82</v>
       </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
       <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
         <v>144</v>
       </c>
-      <c r="M3" t="s">
-        <v>198</v>
-      </c>
       <c r="N3" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="O3" t="s">
-        <v>147</v>
+        <v>289</v>
       </c>
       <c r="P3" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q3" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
         <v>142</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>145</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>143</v>
       </c>
-      <c r="F4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
-        <v>152</v>
-      </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
       <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
         <v>144</v>
       </c>
-      <c r="M4" t="s">
-        <v>198</v>
-      </c>
       <c r="N4" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="O4" t="s">
-        <v>147</v>
+        <v>289</v>
       </c>
       <c r="P4" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q4" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
       <c r="B5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" t="s">
         <v>153</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
         <v>154</v>
       </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
       <c r="J5" t="s">
-        <v>160</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
         <v>144</v>
       </c>
-      <c r="M5" t="s">
-        <v>198</v>
-      </c>
       <c r="N5" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="O5" t="s">
-        <v>162</v>
+        <v>290</v>
       </c>
       <c r="P5" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q5" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
       <c r="B6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N6" t="s">
+        <v>192</v>
+      </c>
+      <c r="O6" t="s">
+        <v>290</v>
+      </c>
+      <c r="P6" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" t="s">
         <v>143</v>
       </c>
-      <c r="F6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" t="s">
-        <v>152</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>161</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" t="s">
-        <v>144</v>
-      </c>
-      <c r="M6" t="s">
-        <v>198</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="G7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>159</v>
+      </c>
+      <c r="L7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" t="s">
+        <v>165</v>
+      </c>
+      <c r="N7" t="s">
+        <v>192</v>
+      </c>
+      <c r="O7" t="s">
         <v>163</v>
       </c>
-      <c r="O6" t="s">
-        <v>162</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q7" t="s">
         <v>62</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R7" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" t="s">
         <v>54</v>
       </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" t="s">
         <v>143</v>
       </c>
-      <c r="F7" t="s">
-        <v>263</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="G8" t="s">
         <v>169</v>
       </c>
-      <c r="M7" t="s">
-        <v>198</v>
-      </c>
-      <c r="N7" t="s">
-        <v>167</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>159</v>
+      </c>
+      <c r="L8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" t="s">
         <v>170</v>
       </c>
-      <c r="P7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="1">
+      <c r="N8" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" t="s">
+        <v>171</v>
+      </c>
+      <c r="P8" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>171</v>
+      </c>
+      <c r="R8" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" t="s">
-        <v>174</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>161</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" t="s">
-        <v>175</v>
-      </c>
-      <c r="M8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" t="s">
-        <v>176</v>
-      </c>
-      <c r="O8" t="s">
-        <v>177</v>
-      </c>
-      <c r="P8" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" t="s">
         <v>54</v>
       </c>
-      <c r="C9" t="s">
-        <v>196</v>
-      </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
         <v>143</v>
       </c>
-      <c r="F9" t="s">
-        <v>262</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
+      <c r="G9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>11</v>
+        <v>172</v>
       </c>
       <c r="L9" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="M9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="N9" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="O9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="P9" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q9" s="1">
+        <v>285</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>171</v>
+      </c>
+      <c r="R9" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
         <v>200</v>
       </c>
-      <c r="D10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" t="s">
-        <v>202</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" t="s">
-        <v>206</v>
-      </c>
-      <c r="J10" t="s">
-        <v>179</v>
-      </c>
       <c r="K10" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="L10" t="s">
-        <v>175</v>
+        <v>11</v>
       </c>
       <c r="M10" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="N10" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O10" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="P10" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q10" t="s">
         <v>62</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="D11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" t="s">
         <v>201</v>
       </c>
-      <c r="E11" t="s">
-        <v>143</v>
-      </c>
-      <c r="F11" t="s">
-        <v>203</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I11" t="s">
-        <v>207</v>
-      </c>
-      <c r="J11" t="s">
-        <v>180</v>
-      </c>
       <c r="K11" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="L11" t="s">
-        <v>175</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="N11" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O11" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="P11" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q11" t="s">
         <v>62</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" t="s">
         <v>143</v>
       </c>
-      <c r="F12" t="s">
-        <v>204</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H12" t="s">
-        <v>208</v>
+      <c r="G12" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="I12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="J12" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="K12" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="L12" t="s">
-        <v>175</v>
+        <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="N12" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O12" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="P12" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q12" t="s">
         <v>62</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" t="s">
         <v>211</v>
       </c>
-      <c r="D13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F13" t="s">
-        <v>216</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H13" t="s">
-        <v>213</v>
-      </c>
-      <c r="I13" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" t="s">
-        <v>182</v>
-      </c>
       <c r="K13" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="L13" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="N13" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O13" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="P13" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q13" t="s">
         <v>62</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R13" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" t="s">
         <v>143</v>
       </c>
-      <c r="F14" t="s">
-        <v>217</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H14" t="s">
-        <v>214</v>
+      <c r="G14" t="s">
+        <v>257</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="I14" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="J14" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="K14" t="s">
-        <v>11</v>
+        <v>177</v>
       </c>
       <c r="L14" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="M14" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="N14" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O14" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="P14" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q14" t="s">
         <v>62</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R14" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>272</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" t="s">
         <v>143</v>
       </c>
-      <c r="F15" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" t="s">
         <v>215</v>
       </c>
-      <c r="I15" t="s">
-        <v>221</v>
-      </c>
-      <c r="J15" t="s">
-        <v>184</v>
-      </c>
-      <c r="K15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" t="s">
-        <v>223</v>
-      </c>
-      <c r="M15" t="s">
-        <v>198</v>
-      </c>
       <c r="N15" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O15" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="P15" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q15" t="s">
         <v>62</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>273</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" t="s">
         <v>212</v>
       </c>
-      <c r="E16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" t="s">
-        <v>220</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
         <v>138</v>
       </c>
-      <c r="I16" t="s">
-        <v>222</v>
-      </c>
       <c r="J16" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="K16" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="L16" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="M16" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="N16" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O16" t="s">
-        <v>199</v>
+        <v>11</v>
       </c>
       <c r="P16" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q16" t="s">
         <v>62</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
       <c r="B17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" t="s">
-        <v>224</v>
-      </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E17" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" t="s">
         <v>143</v>
       </c>
-      <c r="F17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
+      <c r="G17" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>186</v>
+        <v>11</v>
       </c>
       <c r="K17" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="L17" t="s">
-        <v>227</v>
+        <v>11</v>
       </c>
       <c r="M17" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="N17" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="O17" t="s">
-        <v>228</v>
+        <v>11</v>
       </c>
       <c r="P17" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q17" t="s">
         <v>62</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" t="s">
+        <v>222</v>
+      </c>
+      <c r="F18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" t="s">
+        <v>223</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>181</v>
+      </c>
+      <c r="L18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" t="s">
+        <v>191</v>
+      </c>
+      <c r="N18" t="s">
+        <v>192</v>
+      </c>
+      <c r="O18" t="s">
+        <v>171</v>
+      </c>
+      <c r="P18" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>171</v>
+      </c>
+      <c r="R18" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F19" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" t="s">
+        <v>227</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>182</v>
+      </c>
+      <c r="L19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" t="s">
+        <v>228</v>
+      </c>
+      <c r="N19" t="s">
+        <v>192</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>62</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="D18" t="s">
+      <c r="B20" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F18" t="s">
-        <v>231</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="G20" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R20" s="10">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" t="s">
+        <v>237</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>184</v>
+      </c>
+      <c r="L21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" t="s">
+        <v>170</v>
+      </c>
+      <c r="N21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21" t="s">
+        <v>171</v>
+      </c>
+      <c r="P21" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>171</v>
+      </c>
+      <c r="R21" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R22" s="10">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>243</v>
+      </c>
+      <c r="E23" t="s">
+        <v>250</v>
+      </c>
+      <c r="F23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" t="s">
+        <v>244</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>186</v>
+      </c>
+      <c r="L23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" t="s">
+        <v>245</v>
+      </c>
+      <c r="N23" t="s">
+        <v>78</v>
+      </c>
+      <c r="O23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>62</v>
+      </c>
+      <c r="R23" s="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="K18" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" t="s">
-        <v>197</v>
-      </c>
-      <c r="M18" t="s">
-        <v>198</v>
-      </c>
-      <c r="N18" t="s">
-        <v>176</v>
-      </c>
-      <c r="O18" t="s">
-        <v>177</v>
-      </c>
-      <c r="P18" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q18" s="1">
+      <c r="L24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R24" s="10">
         <v>2024</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>232</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D19" t="s">
-        <v>234</v>
-      </c>
-      <c r="E19" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" t="s">
-        <v>235</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" t="s">
-        <v>188</v>
-      </c>
-      <c r="K19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" t="s">
-        <v>236</v>
-      </c>
-      <c r="M19" t="s">
-        <v>198</v>
-      </c>
-      <c r="N19" t="s">
-        <v>11</v>
-      </c>
-      <c r="O19" t="s">
-        <v>199</v>
-      </c>
-      <c r="P19" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="N20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q20" s="10">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>242</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21" t="s">
-        <v>244</v>
-      </c>
-      <c r="E21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" t="s">
-        <v>245</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" t="s">
-        <v>190</v>
-      </c>
-      <c r="K21" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" t="s">
-        <v>175</v>
-      </c>
-      <c r="M21" t="s">
-        <v>78</v>
-      </c>
-      <c r="N21" t="s">
-        <v>176</v>
-      </c>
-      <c r="O21" t="s">
-        <v>177</v>
-      </c>
-      <c r="P21" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q22" s="10">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>251</v>
-      </c>
-      <c r="D23" t="s">
-        <v>258</v>
-      </c>
-      <c r="E23" t="s">
-        <v>143</v>
-      </c>
-      <c r="F23" t="s">
-        <v>252</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>192</v>
-      </c>
-      <c r="K23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" t="s">
-        <v>253</v>
-      </c>
-      <c r="M23" t="s">
-        <v>78</v>
-      </c>
-      <c r="N23" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" t="s">
-        <v>254</v>
-      </c>
-      <c r="P23" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="N24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q24" s="10">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>135</v>
       </c>
       <c r="B25" t="s">
+        <v>282</v>
+      </c>
+      <c r="C25" t="s">
         <v>54</v>
       </c>
-      <c r="C25" t="s">
-        <v>259</v>
-      </c>
       <c r="D25" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E25" t="s">
+        <v>252</v>
+      </c>
+      <c r="F25" t="s">
         <v>143</v>
       </c>
-      <c r="F25" t="s">
-        <v>261</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
-        <v>11</v>
+      <c r="G25" t="s">
+        <v>253</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>194</v>
+        <v>11</v>
       </c>
       <c r="K25" t="s">
-        <v>11</v>
+        <v>188</v>
       </c>
       <c r="L25" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="M25" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="N25" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="O25" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="P25" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q25" s="1">
+        <v>285</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>171</v>
+      </c>
+      <c r="R25" s="1">
         <v>2024</v>
       </c>
     </row>
@@ -4773,16 +4933,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EE7D2B-72B9-4B29-A99A-A2518AB2EE2A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Qatar Report v3 update
</commit_message>
<xml_diff>
--- a/report_outline_v0.xlsx
+++ b/report_outline_v0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4255" documentId="8_{F18DE356-3958-4E61-A81F-20E34B64EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7231B74-B9ED-7A4F-8616-809329BA4A6C}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{6B97058B-77ED-4691-9154-36ED9694847A}"/>
   </bookViews>
   <sheets>
     <sheet name="general_info" sheetId="3" r:id="rId1"/>
@@ -1824,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B32341-F9AC-424D-8D69-9ABCF2FF7D4F}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2971,7 +2971,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:Q17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4599,17 +4599,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4618,7 +4607,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3620e9c0d1a16779aea146adda0186f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2afd3ea0446edf26a13b3c7fc9e6232" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -4867,24 +4856,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EE7D2B-72B9-4B29-A99A-A2518AB2EE2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBF641CD-F15C-42E5-B454-EB7169F6F499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4892,7 +4875,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87354EAB-4CC7-4750-AE59-FEDEECBA27EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4909,4 +4892,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1EE7D2B-72B9-4B29-A99A-A2518AB2EE2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>